<commit_message>
Logic tree input file updated
</commit_message>
<xml_diff>
--- a/Database/Combined Finalize logic tree/Subaru_Impreza Outback Forester legacy_Coolant leak.xlsx
+++ b/Database/Combined Finalize logic tree/Subaru_Impreza Outback Forester legacy_Coolant leak.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26026"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26130"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Sahil\Documents\Shreyash_files\Projects\Amberflux RaH Project\Database\Combined Finalize logic tree\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{3EE3ABB9-6AEC-4BA4-AB2F-32195D905BEE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7EE5D080-5E81-4966-8981-B6111344E0B2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="6252" yWindow="0" windowWidth="16500" windowHeight="12360" xr2:uid="{FD2D2D68-9630-4025-9DFF-9718CDED2B1C}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" xr2:uid="{FD2D2D68-9630-4025-9DFF-9718CDED2B1C}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="27">
   <si>
     <t>Node1</t>
   </si>
@@ -495,10 +495,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EB3682B1-F553-40C8-96BB-422AFBEF843B}">
-  <dimension ref="A1:C21"/>
+  <dimension ref="A1:C23"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A21" workbookViewId="0">
-      <selection activeCell="A21" sqref="A21"/>
+    <sheetView tabSelected="1" topLeftCell="A23" workbookViewId="0">
+      <selection activeCell="B23" sqref="B23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -640,10 +640,10 @@
         <v>14</v>
       </c>
       <c r="B13" t="s">
-        <v>17</v>
+        <v>11</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>18</v>
+        <v>12</v>
       </c>
     </row>
     <row r="14" spans="1:3" ht="230.4" x14ac:dyDescent="0.3">
@@ -651,7 +651,7 @@
         <v>14</v>
       </c>
       <c r="B14" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="C14" s="1" t="s">
         <v>18</v>
@@ -662,32 +662,32 @@
         <v>14</v>
       </c>
       <c r="B15" t="s">
-        <v>15</v>
+        <v>19</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="16" spans="1:3" ht="187.2" x14ac:dyDescent="0.3">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" ht="230.4" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>14</v>
       </c>
       <c r="B16" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="17" spans="1:3" ht="230.4" x14ac:dyDescent="0.3">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" ht="187.2" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="B17" t="s">
         <v>13</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
     </row>
     <row r="18" spans="1:3" ht="230.4" x14ac:dyDescent="0.3">
@@ -695,42 +695,64 @@
         <v>16</v>
       </c>
       <c r="B18" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>22</v>
+        <v>12</v>
       </c>
     </row>
     <row r="19" spans="1:3" ht="230.4" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
-        <v>23</v>
+        <v>16</v>
       </c>
       <c r="B19" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
     </row>
     <row r="20" spans="1:3" ht="230.4" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
-        <v>23</v>
+        <v>16</v>
       </c>
       <c r="B20" t="s">
         <v>15</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="21" spans="1:3" ht="216" x14ac:dyDescent="0.3">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" ht="230.4" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>23</v>
       </c>
       <c r="B21" t="s">
+        <v>11</v>
+      </c>
+      <c r="C21" s="1" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" ht="230.4" x14ac:dyDescent="0.3">
+      <c r="A22" t="s">
+        <v>23</v>
+      </c>
+      <c r="B22" t="s">
+        <v>15</v>
+      </c>
+      <c r="C22" s="1" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" ht="216" x14ac:dyDescent="0.3">
+      <c r="A23" t="s">
+        <v>23</v>
+      </c>
+      <c r="B23" t="s">
         <v>13</v>
       </c>
-      <c r="C21" s="1" t="s">
+      <c r="C23" s="1" t="s">
         <v>25</v>
       </c>
     </row>

</xml_diff>